<commit_message>
actualizacion messageHeader y otros
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-BundleReferenciaLE.xlsx
+++ b/docs/StructureDefinition-BundleReferenciaLE.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AN$209</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6346" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7486" uniqueCount="462">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-13T10:57:49-03:00</t>
+    <t>2023-02-14T08:51:49-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -563,7 +563,7 @@
     <t>Bundle.entry</t>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
   </si>
   <si>
     <t>Entry in the bundle - will have a resource or information</t>
@@ -1200,6 +1200,115 @@
   </si>
   <si>
     <t>Bundle.entry:practitioner.response.outcome</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole</t>
+  </si>
+  <si>
+    <t>practitionerRole</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.link</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.fullUrl</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.resource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PractitionerRole {http://minsal.cl/listaespera/StructureDefinition/PractitionerRoleLE}
+</t>
+  </si>
+  <si>
+    <t>Roles/organizations the practitioner is associated with</t>
+  </si>
+  <si>
+    <t>A specific set of Roles/Locations/specialties/services that a practitioner may perform at an organization for a period of time.</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.search</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.search.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.search.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.search.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.search.mode</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.search.score</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.method</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.url</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.ifNoneMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.ifModifiedSince</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.ifMatch</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.request.ifNoneExist</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response.id</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response.extension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response.modifierExtension</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response.status</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response.location</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response.etag</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response.lastModified</t>
+  </si>
+  <si>
+    <t>Bundle.entry:practitionerRole.response.outcome</t>
   </si>
   <si>
     <t>Bundle.entry:organization</t>
@@ -1652,7 +1761,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN177"/>
+  <dimension ref="A1:AN209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1661,9 +1770,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="52.84765625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="53.2890625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="38.1796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="15.1171875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="15.55859375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="42.984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -1671,7 +1780,7 @@
     <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="77.08984375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="77.26171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -18033,10 +18142,10 @@
       </c>
       <c r="E145" s="2"/>
       <c r="F145" t="s" s="2">
-        <v>382</v>
+        <v>84</v>
       </c>
       <c r="G145" t="s" s="2">
-        <v>382</v>
+        <v>84</v>
       </c>
       <c r="H145" t="s" s="2">
         <v>75</v>
@@ -18134,7 +18243,7 @@
     </row>
     <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B146" t="s" s="2">
         <v>179</v>
@@ -18246,7 +18355,7 @@
     </row>
     <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B147" t="s" s="2">
         <v>180</v>
@@ -18360,7 +18469,7 @@
     </row>
     <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B148" t="s" s="2">
         <v>181</v>
@@ -18476,7 +18585,7 @@
     </row>
     <row r="149" hidden="true">
       <c r="A149" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B149" t="s" s="2">
         <v>182</v>
@@ -18588,7 +18697,7 @@
     </row>
     <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B150" t="s" s="2">
         <v>185</v>
@@ -18702,7 +18811,7 @@
     </row>
     <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B151" t="s" s="2">
         <v>189</v>
@@ -18728,13 +18837,13 @@
         <v>75</v>
       </c>
       <c r="K151" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="L151" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="L151" t="s" s="2">
+      <c r="M151" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="M151" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="N151" s="2"/>
       <c r="O151" s="2"/>
@@ -18797,13 +18906,13 @@
         <v>75</v>
       </c>
       <c r="AJ151" t="s" s="2">
-        <v>392</v>
+        <v>274</v>
       </c>
       <c r="AK151" t="s" s="2">
-        <v>393</v>
+        <v>353</v>
       </c>
       <c r="AL151" t="s" s="2">
-        <v>394</v>
+        <v>354</v>
       </c>
       <c r="AM151" t="s" s="2">
         <v>75</v>
@@ -18814,7 +18923,7 @@
     </row>
     <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B152" t="s" s="2">
         <v>193</v>
@@ -18926,7 +19035,7 @@
     </row>
     <row r="153" hidden="true">
       <c r="A153" t="s" s="2">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B153" t="s" s="2">
         <v>197</v>
@@ -19038,7 +19147,7 @@
     </row>
     <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B154" t="s" s="2">
         <v>198</v>
@@ -19152,7 +19261,7 @@
     </row>
     <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B155" t="s" s="2">
         <v>199</v>
@@ -19268,7 +19377,7 @@
     </row>
     <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B156" t="s" s="2">
         <v>200</v>
@@ -19382,7 +19491,7 @@
     </row>
     <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B157" t="s" s="2">
         <v>206</v>
@@ -19496,7 +19605,7 @@
     </row>
     <row r="158" hidden="true">
       <c r="A158" t="s" s="2">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B158" t="s" s="2">
         <v>211</v>
@@ -19608,7 +19717,7 @@
     </row>
     <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B159" t="s" s="2">
         <v>215</v>
@@ -19720,7 +19829,7 @@
     </row>
     <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B160" t="s" s="2">
         <v>216</v>
@@ -19834,7 +19943,7 @@
     </row>
     <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B161" t="s" s="2">
         <v>217</v>
@@ -19950,7 +20059,7 @@
     </row>
     <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B162" t="s" s="2">
         <v>218</v>
@@ -20062,7 +20171,7 @@
     </row>
     <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B163" t="s" s="2">
         <v>223</v>
@@ -20176,7 +20285,7 @@
     </row>
     <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B164" t="s" s="2">
         <v>227</v>
@@ -20288,7 +20397,7 @@
     </row>
     <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B165" t="s" s="2">
         <v>230</v>
@@ -20400,7 +20509,7 @@
     </row>
     <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B166" t="s" s="2">
         <v>232</v>
@@ -20512,7 +20621,7 @@
     </row>
     <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B167" t="s" s="2">
         <v>235</v>
@@ -20624,7 +20733,7 @@
     </row>
     <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B168" t="s" s="2">
         <v>238</v>
@@ -20736,7 +20845,7 @@
     </row>
     <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B169" t="s" s="2">
         <v>242</v>
@@ -20848,7 +20957,7 @@
     </row>
     <row r="170" hidden="true">
       <c r="A170" t="s" s="2">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B170" t="s" s="2">
         <v>243</v>
@@ -20962,7 +21071,7 @@
     </row>
     <row r="171" hidden="true">
       <c r="A171" t="s" s="2">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B171" t="s" s="2">
         <v>244</v>
@@ -21078,7 +21187,7 @@
     </row>
     <row r="172" hidden="true">
       <c r="A172" t="s" s="2">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B172" t="s" s="2">
         <v>245</v>
@@ -21190,7 +21299,7 @@
     </row>
     <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B173" t="s" s="2">
         <v>248</v>
@@ -21302,7 +21411,7 @@
     </row>
     <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B174" t="s" s="2">
         <v>251</v>
@@ -21416,7 +21525,7 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B175" t="s" s="2">
         <v>255</v>
@@ -21530,7 +21639,7 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B176" t="s" s="2">
         <v>259</v>
@@ -21644,21 +21753,23 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B177" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="C177" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="C177" t="s" s="2">
+        <v>417</v>
+      </c>
       <c r="D177" t="s" s="2">
         <v>75</v>
       </c>
       <c r="E177" s="2"/>
       <c r="F177" t="s" s="2">
-        <v>76</v>
+        <v>418</v>
       </c>
       <c r="G177" t="s" s="2">
-        <v>84</v>
+        <v>418</v>
       </c>
       <c r="H177" t="s" s="2">
         <v>75</v>
@@ -21670,20 +21781,16 @@
         <v>85</v>
       </c>
       <c r="K177" t="s" s="2">
-        <v>421</v>
+        <v>142</v>
       </c>
       <c r="L177" t="s" s="2">
-        <v>422</v>
+        <v>174</v>
       </c>
       <c r="M177" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="N177" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="O177" t="s" s="2">
-        <v>425</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="N177" s="2"/>
+      <c r="O177" s="2"/>
       <c r="P177" t="s" s="2">
         <v>75</v>
       </c>
@@ -21731,35 +21838,3661 @@
         <v>75</v>
       </c>
       <c r="AF177" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="AG177" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH177" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI177" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ177" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="AK177" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL177" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM177" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN177" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="178" hidden="true">
+      <c r="A178" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="B178" t="s" s="2">
+        <v>179</v>
+      </c>
+      <c r="C178" s="2"/>
+      <c r="D178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E178" s="2"/>
+      <c r="F178" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G178" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K178" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L178" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="M178" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="N178" s="2"/>
+      <c r="O178" s="2"/>
+      <c r="P178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q178" s="2"/>
+      <c r="R178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF178" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="AG178" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH178" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL178" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AM178" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN178" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="179" hidden="true">
+      <c r="A179" t="s" s="2">
         <v>420</v>
       </c>
-      <c r="AG177" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AH177" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AI177" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AJ177" t="s" s="2">
+      <c r="B179" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="C179" s="2"/>
+      <c r="D179" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="E179" s="2"/>
+      <c r="F179" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G179" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K179" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L179" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="M179" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="N179" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O179" s="2"/>
+      <c r="P179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q179" s="2"/>
+      <c r="R179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF179" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AG179" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH179" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ179" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL179" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AM179" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN179" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="180" hidden="true">
+      <c r="A180" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="B180" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="C180" s="2"/>
+      <c r="D180" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="E180" s="2"/>
+      <c r="F180" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G180" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I180" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="J180" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K180" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L180" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="M180" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="N180" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O180" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="P180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q180" s="2"/>
+      <c r="R180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF180" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AG180" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH180" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ180" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL180" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AM180" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN180" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="181" hidden="true">
+      <c r="A181" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="B181" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="C181" s="2"/>
+      <c r="D181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E181" s="2"/>
+      <c r="F181" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G181" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J181" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K181" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="L181" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="M181" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="N181" s="2"/>
+      <c r="O181" s="2"/>
+      <c r="P181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q181" s="2"/>
+      <c r="R181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF181" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="AG181" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH181" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ181" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="AK177" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AL177" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AM177" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AN177" t="s" s="2">
+      <c r="AK181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM181" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN181" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="182" hidden="true">
+      <c r="A182" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="B182" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="C182" s="2"/>
+      <c r="D182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E182" s="2"/>
+      <c r="F182" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G182" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J182" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K182" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L182" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="M182" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="N182" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="O182" s="2"/>
+      <c r="P182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q182" s="2"/>
+      <c r="R182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF182" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="AG182" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH182" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ182" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM182" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN182" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="183" hidden="true">
+      <c r="A183" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="B183" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="C183" s="2"/>
+      <c r="D183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E183" s="2"/>
+      <c r="F183" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G183" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K183" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="L183" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="M183" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="N183" s="2"/>
+      <c r="O183" s="2"/>
+      <c r="P183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q183" s="2"/>
+      <c r="R183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF183" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="AG183" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH183" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ183" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="AK183" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="AL183" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="AM183" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN183" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="184" hidden="true">
+      <c r="A184" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="B184" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="C184" s="2"/>
+      <c r="D184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E184" s="2"/>
+      <c r="F184" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G184" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J184" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K184" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="L184" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="M184" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="N184" s="2"/>
+      <c r="O184" s="2"/>
+      <c r="P184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q184" s="2"/>
+      <c r="R184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF184" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="AG184" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH184" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI184" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="AJ184" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM184" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN184" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="185" hidden="true">
+      <c r="A185" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="B185" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="C185" s="2"/>
+      <c r="D185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E185" s="2"/>
+      <c r="F185" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G185" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K185" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L185" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="M185" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="N185" s="2"/>
+      <c r="O185" s="2"/>
+      <c r="P185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q185" s="2"/>
+      <c r="R185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF185" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="AG185" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH185" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL185" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AM185" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN185" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="186" hidden="true">
+      <c r="A186" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="B186" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="C186" s="2"/>
+      <c r="D186" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="E186" s="2"/>
+      <c r="F186" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G186" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K186" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L186" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="M186" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="N186" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O186" s="2"/>
+      <c r="P186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q186" s="2"/>
+      <c r="R186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF186" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AG186" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH186" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ186" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL186" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AM186" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN186" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="187" hidden="true">
+      <c r="A187" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="B187" t="s" s="2">
+        <v>199</v>
+      </c>
+      <c r="C187" s="2"/>
+      <c r="D187" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="E187" s="2"/>
+      <c r="F187" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G187" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I187" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="J187" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K187" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L187" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="M187" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="N187" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O187" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="P187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q187" s="2"/>
+      <c r="R187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF187" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AG187" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH187" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ187" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL187" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AM187" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN187" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="188" hidden="true">
+      <c r="A188" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="B188" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="C188" s="2"/>
+      <c r="D188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E188" s="2"/>
+      <c r="F188" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G188" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J188" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K188" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L188" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="M188" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="N188" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="O188" s="2"/>
+      <c r="P188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q188" s="2"/>
+      <c r="R188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X188" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="Y188" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="Z188" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="AA188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF188" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="AG188" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH188" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ188" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM188" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN188" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="189" hidden="true">
+      <c r="A189" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="B189" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="C189" s="2"/>
+      <c r="D189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E189" s="2"/>
+      <c r="F189" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G189" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J189" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K189" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="L189" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="M189" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N189" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="O189" s="2"/>
+      <c r="P189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q189" s="2"/>
+      <c r="R189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF189" t="s" s="2">
+        <v>206</v>
+      </c>
+      <c r="AG189" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH189" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ189" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM189" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN189" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="190" hidden="true">
+      <c r="A190" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="B190" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="C190" s="2"/>
+      <c r="D190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E190" s="2"/>
+      <c r="F190" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G190" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J190" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K190" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="L190" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="M190" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="N190" s="2"/>
+      <c r="O190" s="2"/>
+      <c r="P190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q190" s="2"/>
+      <c r="R190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF190" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AG190" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH190" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI190" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="AJ190" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM190" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN190" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="191" hidden="true">
+      <c r="A191" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="B191" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="C191" s="2"/>
+      <c r="D191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E191" s="2"/>
+      <c r="F191" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G191" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K191" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L191" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="M191" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="N191" s="2"/>
+      <c r="O191" s="2"/>
+      <c r="P191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q191" s="2"/>
+      <c r="R191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF191" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="AG191" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH191" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL191" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AM191" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN191" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="192" hidden="true">
+      <c r="A192" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="B192" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="C192" s="2"/>
+      <c r="D192" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="E192" s="2"/>
+      <c r="F192" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G192" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K192" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L192" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="M192" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="N192" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O192" s="2"/>
+      <c r="P192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q192" s="2"/>
+      <c r="R192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF192" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AG192" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH192" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ192" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL192" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AM192" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN192" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="193" hidden="true">
+      <c r="A193" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="B193" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="C193" s="2"/>
+      <c r="D193" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="E193" s="2"/>
+      <c r="F193" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G193" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I193" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="J193" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K193" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L193" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="M193" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="N193" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O193" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="P193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q193" s="2"/>
+      <c r="R193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF193" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AG193" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH193" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ193" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL193" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AM193" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN193" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="194" hidden="true">
+      <c r="A194" t="s" s="2">
+        <v>441</v>
+      </c>
+      <c r="B194" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="C194" s="2"/>
+      <c r="D194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E194" s="2"/>
+      <c r="F194" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G194" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J194" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K194" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L194" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="M194" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="N194" s="2"/>
+      <c r="O194" s="2"/>
+      <c r="P194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q194" s="2"/>
+      <c r="R194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X194" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="Y194" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="Z194" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="AA194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF194" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="AG194" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AH194" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ194" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM194" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN194" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="195" hidden="true">
+      <c r="A195" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="B195" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="C195" s="2"/>
+      <c r="D195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E195" s="2"/>
+      <c r="F195" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G195" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J195" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K195" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L195" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="M195" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="N195" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="O195" s="2"/>
+      <c r="P195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q195" s="2"/>
+      <c r="R195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF195" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="AG195" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AH195" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ195" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM195" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN195" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="196" hidden="true">
+      <c r="A196" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="B196" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="C196" s="2"/>
+      <c r="D196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E196" s="2"/>
+      <c r="F196" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G196" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J196" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K196" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L196" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="M196" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="N196" s="2"/>
+      <c r="O196" s="2"/>
+      <c r="P196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q196" s="2"/>
+      <c r="R196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF196" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AG196" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH196" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ196" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM196" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN196" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="197" hidden="true">
+      <c r="A197" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="B197" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="C197" s="2"/>
+      <c r="D197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E197" s="2"/>
+      <c r="F197" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G197" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J197" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K197" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="L197" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="M197" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="N197" s="2"/>
+      <c r="O197" s="2"/>
+      <c r="P197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q197" s="2"/>
+      <c r="R197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF197" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="AG197" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH197" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ197" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM197" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN197" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="198" hidden="true">
+      <c r="A198" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="B198" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="C198" s="2"/>
+      <c r="D198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E198" s="2"/>
+      <c r="F198" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G198" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J198" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K198" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L198" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="M198" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="N198" s="2"/>
+      <c r="O198" s="2"/>
+      <c r="P198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q198" s="2"/>
+      <c r="R198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF198" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AG198" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH198" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ198" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM198" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN198" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="199" hidden="true">
+      <c r="A199" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="B199" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="C199" s="2"/>
+      <c r="D199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E199" s="2"/>
+      <c r="F199" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G199" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J199" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K199" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L199" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="M199" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="N199" s="2"/>
+      <c r="O199" s="2"/>
+      <c r="P199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q199" s="2"/>
+      <c r="R199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF199" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="AG199" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH199" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ199" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM199" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN199" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="200" hidden="true">
+      <c r="A200" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="B200" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="C200" s="2"/>
+      <c r="D200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E200" s="2"/>
+      <c r="F200" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G200" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J200" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K200" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="L200" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="M200" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="N200" s="2"/>
+      <c r="O200" s="2"/>
+      <c r="P200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q200" s="2"/>
+      <c r="R200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF200" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AG200" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH200" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI200" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AJ200" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM200" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN200" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="201" hidden="true">
+      <c r="A201" t="s" s="2">
+        <v>448</v>
+      </c>
+      <c r="B201" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="C201" s="2"/>
+      <c r="D201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E201" s="2"/>
+      <c r="F201" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G201" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K201" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L201" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="M201" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="N201" s="2"/>
+      <c r="O201" s="2"/>
+      <c r="P201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q201" s="2"/>
+      <c r="R201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF201" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="AG201" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH201" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL201" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AM201" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN201" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="202" hidden="true">
+      <c r="A202" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="B202" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="C202" s="2"/>
+      <c r="D202" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="E202" s="2"/>
+      <c r="F202" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G202" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K202" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L202" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="M202" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="N202" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O202" s="2"/>
+      <c r="P202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q202" s="2"/>
+      <c r="R202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF202" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="AG202" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH202" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ202" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL202" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="AM202" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN202" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="203" hidden="true">
+      <c r="A203" t="s" s="2">
+        <v>450</v>
+      </c>
+      <c r="B203" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="C203" s="2"/>
+      <c r="D203" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="E203" s="2"/>
+      <c r="F203" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G203" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="H203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I203" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="J203" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K203" t="s" s="2">
+        <v>154</v>
+      </c>
+      <c r="L203" t="s" s="2">
+        <v>162</v>
+      </c>
+      <c r="M203" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="N203" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="O203" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="P203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q203" s="2"/>
+      <c r="R203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF203" t="s" s="2">
+        <v>165</v>
+      </c>
+      <c r="AG203" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH203" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AI203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ203" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="AK203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL203" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="AM203" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN203" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="204" hidden="true">
+      <c r="A204" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="B204" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="C204" s="2"/>
+      <c r="D204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E204" s="2"/>
+      <c r="F204" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="G204" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J204" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K204" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L204" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="M204" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="N204" s="2"/>
+      <c r="O204" s="2"/>
+      <c r="P204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q204" s="2"/>
+      <c r="R204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF204" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="AG204" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AH204" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ204" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM204" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN204" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="205" hidden="true">
+      <c r="A205" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="B205" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="C205" s="2"/>
+      <c r="D205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E205" s="2"/>
+      <c r="F205" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G205" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J205" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K205" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="L205" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="M205" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="N205" s="2"/>
+      <c r="O205" s="2"/>
+      <c r="P205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q205" s="2"/>
+      <c r="R205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF205" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="AG205" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH205" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ205" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM205" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN205" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="206" hidden="true">
+      <c r="A206" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="B206" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="C206" s="2"/>
+      <c r="D206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E206" s="2"/>
+      <c r="F206" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G206" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J206" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K206" t="s" s="2">
+        <v>147</v>
+      </c>
+      <c r="L206" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="M206" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="N206" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="O206" s="2"/>
+      <c r="P206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q206" s="2"/>
+      <c r="R206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF206" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="AG206" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH206" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ206" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM206" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN206" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="207" hidden="true">
+      <c r="A207" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="B207" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="C207" s="2"/>
+      <c r="D207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E207" s="2"/>
+      <c r="F207" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G207" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J207" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K207" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="L207" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="M207" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="N207" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="O207" s="2"/>
+      <c r="P207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q207" s="2"/>
+      <c r="R207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF207" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AG207" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH207" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ207" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM207" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN207" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="208" hidden="true">
+      <c r="A208" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="B208" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="C208" s="2"/>
+      <c r="D208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E208" s="2"/>
+      <c r="F208" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G208" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J208" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K208" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="L208" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="M208" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="N208" t="s" s="2">
+        <v>262</v>
+      </c>
+      <c r="O208" s="2"/>
+      <c r="P208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q208" s="2"/>
+      <c r="R208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF208" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="AG208" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH208" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM208" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN208" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="209" hidden="true">
+      <c r="A209" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="B209" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="C209" s="2"/>
+      <c r="D209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="E209" s="2"/>
+      <c r="F209" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="G209" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="I209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J209" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K209" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="L209" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="M209" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="N209" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="O209" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="P209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Q209" s="2"/>
+      <c r="R209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="S209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF209" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="AG209" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AH209" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AJ209" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="AK209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AL209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AM209" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AN209" t="s" s="2">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN177">
+  <autoFilter ref="A1:AN209">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -21769,7 +25502,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI176">
+  <conditionalFormatting sqref="A2:AI208">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>